<commit_message>
Updated with 2019 calibration results.
</commit_message>
<xml_diff>
--- a/InductorSet.xlsx
+++ b/InductorSet.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\KJ\PycharmProjects\UniversalBridge3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E062F7C0-EFEA-4927-8395-EA1E9088A6F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815937BA-FD0D-4627-834D-A7D9648A426B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commentary" sheetId="24" r:id="rId1"/>
     <sheet name="pyUBreadings" sheetId="21" r:id="rId2"/>
     <sheet name="pyUBresults" sheetId="22" r:id="rId3"/>
     <sheet name="pyReport" sheetId="29" r:id="rId4"/>
-    <sheet name="Room Conditions" sheetId="25" r:id="rId5"/>
-    <sheet name="Conditions" sheetId="18" r:id="rId6"/>
+    <sheet name="exampleU" sheetId="30" r:id="rId5"/>
+    <sheet name="Room Conditions" sheetId="25" r:id="rId6"/>
+    <sheet name="Conditions" sheetId="18" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="alpha">#REF!</definedName>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="128">
   <si>
     <t>Label</t>
   </si>
@@ -372,6 +373,126 @@
   <si>
     <t>You should check that the input data listed in 'pyUBresults' matches the input data in 'pyUBreadings', just in case the wrong file names are enterd in 'calculate_imp.py'.</t>
   </si>
+  <si>
+    <t>Budget for L8 1591.5</t>
+  </si>
+  <si>
+    <t>ureal(60.08704790830853,0.1713140491986457,20.451673221652594)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuttempL8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amp_phase_err </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rtempcoL8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adialresureal(62.0,10.0,10.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adialresureal(600890.0,10.0,10.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adial_lin62 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adial_lin600890 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amperr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4Aacdc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1acdc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2acdc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1alpha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1stab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4Aalpha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2alpha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4Astab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2stab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cal_temp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2err </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1err </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4Aerr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuttempL0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rtempcoL0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1err </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1alpha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1stab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bdial_lin0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bdialresureal(0.0,1.0,10.0, label='Bdial_lin0') </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bdial_lin788633 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bdialresureal(788633.0,1.0,10.0) </t>
+  </si>
+  <si>
+    <t>ureal(0.0788795386314938,3.031875053076101e-06,27.783955120984952)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xtempcoL8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">xtempcoL0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bdialres0.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bdialres788633.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adialres62.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adialres600890.0 </t>
+  </si>
 </sst>
 </file>
 
@@ -381,13 +502,13 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0E+00"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="172" formatCode="0.0000\ \ \ \ \ "/>
-    <numFmt numFmtId="175" formatCode="0.00\ \ \ \ \ \ "/>
-    <numFmt numFmtId="176" formatCode="0.000\ \ \ \ \ "/>
-    <numFmt numFmtId="177" formatCode="0.0\ \ \ \ \ \ "/>
+    <numFmt numFmtId="167" formatCode="0.0E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="170" formatCode="0.0000\ \ \ \ \ "/>
+    <numFmt numFmtId="171" formatCode="0.00\ \ \ \ \ \ "/>
+    <numFmt numFmtId="172" formatCode="0.000\ \ \ \ \ "/>
+    <numFmt numFmtId="173" formatCode="0.0\ \ \ \ \ \ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -604,7 +725,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -658,14 +779,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -696,19 +817,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1126,7 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3147,7 +3268,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q3" sqref="Q3"/>
+      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3340,10 +3461,10 @@
         <v>0</v>
       </c>
       <c r="V2">
-        <v>1.257071026042052E-7</v>
+        <v>1.257071026042056E-7</v>
       </c>
       <c r="W2">
-        <v>1.2570710275100531E-3</v>
+        <v>1.25707102751006E-3</v>
       </c>
       <c r="X2" s="10">
         <f t="shared" ref="X2:X18" si="0">Q2/V2</f>
@@ -3442,36 +3563,36 @@
         <v>10</v>
       </c>
       <c r="P3">
-        <v>1.015108976635559E-2</v>
+        <v>1.0151092810620941E-2</v>
       </c>
       <c r="Q3">
-        <v>9.0104883355186138E-7</v>
+        <v>9.0104910728435296E-7</v>
       </c>
       <c r="R3">
-        <v>2.0142871658839789</v>
+        <v>2.0142871649350962</v>
       </c>
       <c r="S3">
-        <v>19.40867211366508</v>
+        <v>19.40869540284854</v>
       </c>
       <c r="T3">
-        <v>0.11511800312028141</v>
+        <v>0.1151181411798763</v>
       </c>
       <c r="U3">
-        <v>2.0839745776262251</v>
+        <v>2.083974578081909</v>
       </c>
       <c r="V3">
-        <v>1.9072482554206981E-7</v>
+        <v>1.9072485967089009E-7</v>
       </c>
       <c r="W3">
-        <v>1.638460710927572E-3</v>
+        <v>1.6384609536414609E-3</v>
       </c>
       <c r="X3" s="10">
         <f t="shared" si="0"/>
-        <v>4.7243395346722146</v>
+        <v>4.7243401245080481</v>
       </c>
       <c r="Y3" s="10">
         <f t="shared" si="1"/>
-        <v>70.259849596949039</v>
+        <v>70.259923450740487</v>
       </c>
       <c r="Z3" t="str">
         <f>A3&amp;B3</f>
@@ -3482,30 +3603,30 @@
       </c>
       <c r="AB3" s="42">
         <f t="shared" ref="AB3:AB23" si="2">AA3*S3</f>
-        <v>19408.672113665081</v>
+        <v>19408.695402848542</v>
       </c>
       <c r="AC3" s="28">
         <f t="shared" ref="AC3:AC23" si="3">AA3*T3</f>
-        <v>115.1180031202814</v>
+        <v>115.1181411798763</v>
       </c>
       <c r="AD3" s="10">
         <f t="shared" ref="AD3:AD23" si="4">U3</f>
-        <v>2.0839745776262251</v>
+        <v>2.083974578081909</v>
       </c>
       <c r="AE3" s="25">
         <v>1000000</v>
       </c>
       <c r="AF3" s="25">
         <f t="shared" ref="AF3:AF23" si="5">AE3*P3</f>
-        <v>10151.08976635559</v>
+        <v>10151.092810620941</v>
       </c>
       <c r="AG3" s="10">
         <f t="shared" ref="AG3:AG23" si="6">AE3*Q3</f>
-        <v>0.90104883355186138</v>
+        <v>0.90104910728435295</v>
       </c>
       <c r="AH3" s="3">
         <f t="shared" ref="AH3:AH23" si="7">R3</f>
-        <v>2.0142871658839789</v>
+        <v>2.0142871649350962</v>
       </c>
       <c r="AI3" s="3">
         <f t="shared" ref="AI3:AI23" si="8">B3</f>
@@ -3560,36 +3681,36 @@
         <v>10</v>
       </c>
       <c r="P4">
-        <v>1.9991315536319089E-2</v>
+        <v>1.9991321531623099E-2</v>
       </c>
       <c r="Q4">
-        <v>1.6250152697106631E-6</v>
+        <v>1.625015760574233E-6</v>
       </c>
       <c r="R4">
-        <v>2.036544885767873</v>
+        <v>2.0365448849629679</v>
       </c>
       <c r="S4">
-        <v>27.90327264714842</v>
+        <v>27.903306129317219</v>
       </c>
       <c r="T4">
-        <v>0.1654960414164828</v>
+        <v>0.16549623979952069</v>
       </c>
       <c r="U4">
-        <v>2.083965226242531</v>
+        <v>2.08396522709607</v>
       </c>
       <c r="V4">
-        <v>3.0807976707608129E-7</v>
+        <v>3.0807984636095379E-7</v>
       </c>
       <c r="W4">
-        <v>2.3936220487426468E-3</v>
+        <v>2.393622626000457E-3</v>
       </c>
       <c r="X4" s="10">
         <f t="shared" si="0"/>
-        <v>5.2746575509756228</v>
+        <v>5.2746577868333695</v>
       </c>
       <c r="Y4" s="10">
         <f t="shared" si="1"/>
-        <v>69.140423193969468</v>
+        <v>69.140489399555463</v>
       </c>
       <c r="Z4" t="str">
         <f t="shared" ref="Z4:Z17" si="9">A4&amp;B4</f>
@@ -3600,30 +3721,30 @@
       </c>
       <c r="AB4" s="42">
         <f t="shared" si="2"/>
-        <v>27903.27264714842</v>
+        <v>27903.306129317218</v>
       </c>
       <c r="AC4" s="28">
         <f t="shared" si="3"/>
-        <v>165.4960414164828</v>
+        <v>165.49623979952068</v>
       </c>
       <c r="AD4" s="10">
         <f t="shared" si="4"/>
-        <v>2.083965226242531</v>
+        <v>2.08396522709607</v>
       </c>
       <c r="AE4" s="25">
         <v>1000000</v>
       </c>
       <c r="AF4" s="25">
         <f t="shared" si="5"/>
-        <v>19991.315536319089</v>
+        <v>19991.3215316231</v>
       </c>
       <c r="AG4" s="10">
         <f t="shared" si="6"/>
-        <v>1.625015269710663</v>
+        <v>1.625015760574233</v>
       </c>
       <c r="AH4" s="3">
         <f t="shared" si="7"/>
-        <v>2.036544885767873</v>
+        <v>2.0365448849629679</v>
       </c>
       <c r="AI4" s="3">
         <f t="shared" si="8"/>
@@ -3678,36 +3799,36 @@
         <v>10</v>
       </c>
       <c r="P5">
-        <v>2.9269025503287381E-2</v>
+        <v>2.926903428093414E-2</v>
       </c>
       <c r="Q5">
-        <v>2.3374466022814501E-6</v>
+        <v>2.3374473066053911E-6</v>
       </c>
       <c r="R5">
-        <v>2.0431969812943169</v>
+        <v>2.0431969807060941</v>
       </c>
       <c r="S5">
-        <v>34.345528088235419</v>
+        <v>34.345569300704767</v>
       </c>
       <c r="T5">
-        <v>0.2037388544346653</v>
+        <v>0.20373909855685571</v>
       </c>
       <c r="U5">
-        <v>2.0838364610538198</v>
+        <v>2.083836462257691</v>
       </c>
       <c r="V5">
-        <v>4.299892838504603E-7</v>
+        <v>4.2998940425103522E-7</v>
       </c>
       <c r="W5">
-        <v>3.221532893721942E-3</v>
+        <v>3.2215337773581032E-3</v>
       </c>
       <c r="X5" s="10">
         <f t="shared" si="0"/>
-        <v>5.4360578043948573</v>
+        <v>5.4360579202569124</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" si="1"/>
-        <v>63.242829161144826</v>
+        <v>63.242887592486113</v>
       </c>
       <c r="Z5" t="str">
         <f t="shared" si="9"/>
@@ -3718,30 +3839,30 @@
       </c>
       <c r="AB5" s="42">
         <f t="shared" si="2"/>
-        <v>34345.52808823542</v>
+        <v>34345.569300704767</v>
       </c>
       <c r="AC5" s="28">
         <f t="shared" si="3"/>
-        <v>203.73885443466531</v>
+        <v>203.73909855685571</v>
       </c>
       <c r="AD5" s="10">
         <f t="shared" si="4"/>
-        <v>2.0838364610538198</v>
+        <v>2.083836462257691</v>
       </c>
       <c r="AE5" s="25">
         <v>1000000</v>
       </c>
       <c r="AF5" s="25">
         <f t="shared" si="5"/>
-        <v>29269.025503287383</v>
+        <v>29269.034280934138</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" si="6"/>
-        <v>2.33744660228145</v>
+        <v>2.3374473066053909</v>
       </c>
       <c r="AH5" s="3">
         <f t="shared" si="7"/>
-        <v>2.0431969812943169</v>
+        <v>2.0431969807060941</v>
       </c>
       <c r="AI5" s="3">
         <f t="shared" si="8"/>
@@ -3800,36 +3921,36 @@
         <v>10</v>
       </c>
       <c r="P6">
-        <v>3.9351501144313183E-2</v>
+        <v>3.9351512945648218E-2</v>
       </c>
       <c r="Q6">
-        <v>3.120455472991634E-6</v>
+        <v>3.1204564118696618E-6</v>
       </c>
       <c r="R6">
-        <v>2.0461426234706419</v>
+        <v>2.046142623046403</v>
       </c>
       <c r="S6">
-        <v>40.399956111511642</v>
+        <v>40.400004588913077</v>
       </c>
       <c r="T6">
-        <v>0.23970869198841849</v>
+        <v>0.23970897908311969</v>
       </c>
       <c r="U6">
-        <v>2.0836682469806882</v>
+        <v>2.0836682485476938</v>
       </c>
       <c r="V6">
-        <v>5.6652352024144852E-7</v>
+        <v>5.6652368436797307E-7</v>
       </c>
       <c r="W6">
-        <v>4.1696084769743628E-3</v>
+        <v>4.1696096828390391E-3</v>
       </c>
       <c r="X6" s="10">
         <f t="shared" si="0"/>
-        <v>5.5080775316472597</v>
+        <v>5.5080775931740877</v>
       </c>
       <c r="Y6" s="10">
         <f t="shared" si="1"/>
-        <v>57.489496510799704</v>
+        <v>57.489548738745398</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" si="9"/>
@@ -3840,30 +3961,30 @@
       </c>
       <c r="AB6" s="42">
         <f t="shared" si="2"/>
-        <v>40399.956111511645</v>
+        <v>40400.004588913078</v>
       </c>
       <c r="AC6" s="28">
         <f t="shared" si="3"/>
-        <v>239.70869198841848</v>
+        <v>239.70897908311969</v>
       </c>
       <c r="AD6" s="10">
         <f t="shared" si="4"/>
-        <v>2.0836682469806882</v>
+        <v>2.0836682485476938</v>
       </c>
       <c r="AE6" s="25">
         <v>1000000</v>
       </c>
       <c r="AF6" s="25">
         <f t="shared" si="5"/>
-        <v>39351.501144313181</v>
+        <v>39351.512945648217</v>
       </c>
       <c r="AG6" s="10">
         <f t="shared" si="6"/>
-        <v>3.1204554729916341</v>
+        <v>3.1204564118696618</v>
       </c>
       <c r="AH6" s="3">
         <f t="shared" si="7"/>
-        <v>2.0461426234706419</v>
+        <v>2.046142623046403</v>
       </c>
       <c r="AI6" s="3">
         <f t="shared" si="8"/>
@@ -3919,36 +4040,36 @@
         <v>10</v>
       </c>
       <c r="P7">
-        <v>4.9054898745980548E-2</v>
+        <v>4.9054913457320097E-2</v>
       </c>
       <c r="Q7">
-        <v>3.8775682124120648E-6</v>
+        <v>3.8775693780887246E-6</v>
       </c>
       <c r="R7">
-        <v>2.0475205998446748</v>
+        <v>2.04752059952513</v>
       </c>
       <c r="S7">
-        <v>45.744533951285788</v>
+        <v>45.74458884184385</v>
       </c>
       <c r="T7">
-        <v>0.27148179239964138</v>
+        <v>0.2714821174183315</v>
       </c>
       <c r="U7">
-        <v>2.0835047626907799</v>
+        <v>2.0835047645835121</v>
       </c>
       <c r="V7">
-        <v>6.9967599010946248E-7</v>
+        <v>6.996761958584501E-7</v>
       </c>
       <c r="W7">
-        <v>5.104342454332709E-3</v>
+        <v>5.1043439645979943E-3</v>
       </c>
       <c r="X7" s="10">
         <f t="shared" si="0"/>
-        <v>5.5419483692808003</v>
+        <v>5.5419484056210297</v>
       </c>
       <c r="Y7" s="10">
         <f t="shared" si="1"/>
-        <v>53.18643778871067</v>
+        <v>53.186485726910213</v>
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="9"/>
@@ -3959,30 +4080,30 @@
       </c>
       <c r="AB7" s="42">
         <f t="shared" si="2"/>
-        <v>45744.53395128579</v>
+        <v>45744.588841843848</v>
       </c>
       <c r="AC7" s="28">
         <f t="shared" si="3"/>
-        <v>271.48179239964139</v>
+        <v>271.48211741833148</v>
       </c>
       <c r="AD7" s="10">
         <f t="shared" si="4"/>
-        <v>2.0835047626907799</v>
+        <v>2.0835047645835121</v>
       </c>
       <c r="AE7" s="25">
         <v>1000000</v>
       </c>
       <c r="AF7" s="25">
         <f t="shared" si="5"/>
-        <v>49054.89874598055</v>
+        <v>49054.913457320094</v>
       </c>
       <c r="AG7" s="10">
         <f t="shared" si="6"/>
-        <v>3.877568212412065</v>
+        <v>3.8775693780887246</v>
       </c>
       <c r="AH7" s="3">
         <f t="shared" si="7"/>
-        <v>2.0475205998446748</v>
+        <v>2.04752059952513</v>
       </c>
       <c r="AI7" s="3">
         <f t="shared" si="8"/>
@@ -4041,36 +4162,36 @@
         <v>10</v>
       </c>
       <c r="P8">
-        <v>5.9098366356571043E-2</v>
+        <v>5.9098384079900562E-2</v>
       </c>
       <c r="Q8">
-        <v>4.6630188105605617E-6</v>
+        <v>4.6630202115080383E-6</v>
       </c>
       <c r="R8">
-        <v>2.048321446438941</v>
+        <v>2.048321446196987</v>
       </c>
       <c r="S8">
-        <v>50.843894455198154</v>
+        <v>50.843955464667467</v>
       </c>
       <c r="T8">
-        <v>0.30181722511744519</v>
+        <v>0.3018175863091932</v>
       </c>
       <c r="U8">
-        <v>2.0833352473248459</v>
+        <v>2.0833352495406552</v>
       </c>
       <c r="V8">
-        <v>8.3841572106945654E-7</v>
+        <v>8.3841596962992252E-7</v>
       </c>
       <c r="W8">
-        <v>6.0838474769144653E-3</v>
+        <v>6.0838492985135087E-3</v>
       </c>
       <c r="X8" s="10">
         <f t="shared" si="0"/>
-        <v>5.5617024983889403</v>
+        <v>5.5617025204878896</v>
       </c>
       <c r="Y8" s="10">
         <f t="shared" si="1"/>
-        <v>49.609597588156063</v>
+        <v>49.609642103221965</v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="9"/>
@@ -4081,30 +4202,30 @@
       </c>
       <c r="AB8" s="42">
         <f t="shared" si="2"/>
-        <v>50843.894455198155</v>
+        <v>50843.955464667466</v>
       </c>
       <c r="AC8" s="28">
         <f t="shared" si="3"/>
-        <v>301.81722511744516</v>
+        <v>301.81758630919319</v>
       </c>
       <c r="AD8" s="10">
         <f t="shared" si="4"/>
-        <v>2.0833352473248459</v>
+        <v>2.0833352495406552</v>
       </c>
       <c r="AE8" s="25">
         <v>1000000</v>
       </c>
       <c r="AF8" s="25">
         <f t="shared" si="5"/>
-        <v>59098.366356571045</v>
+        <v>59098.384079900563</v>
       </c>
       <c r="AG8" s="10">
         <f t="shared" si="6"/>
-        <v>4.6630188105605619</v>
+        <v>4.6630202115080381</v>
       </c>
       <c r="AH8" s="3">
         <f t="shared" si="7"/>
-        <v>2.048321446438941</v>
+        <v>2.048321446196987</v>
       </c>
       <c r="AI8" s="3">
         <f t="shared" si="8"/>
@@ -4160,36 +4281,36 @@
         <v>10</v>
       </c>
       <c r="P9">
-        <v>6.8943393114895807E-2</v>
+        <v>6.8943413790703789E-2</v>
       </c>
       <c r="Q9">
-        <v>5.4339667532165236E-6</v>
+        <v>5.4339683850815083E-6</v>
       </c>
       <c r="R9">
-        <v>2.0488037718553329</v>
+        <v>2.048803771669879</v>
       </c>
       <c r="S9">
-        <v>55.530225759636913</v>
+        <v>55.530292392408477</v>
       </c>
       <c r="T9">
-        <v>0.32971272028866228</v>
+        <v>0.32971311471397219</v>
       </c>
       <c r="U9">
-        <v>2.0831716935522779</v>
+        <v>2.083171696071715</v>
       </c>
       <c r="V9">
-        <v>9.7494209841599038E-7</v>
+        <v>9.7494238878317408E-7</v>
       </c>
       <c r="W9">
-        <v>7.0510044568876783E-3</v>
+        <v>7.0510065814065317E-3</v>
       </c>
       <c r="X9" s="10">
         <f t="shared" si="0"/>
-        <v>5.5736302310108545</v>
+        <v>5.573630244822616</v>
       </c>
       <c r="Y9" s="10">
         <f t="shared" si="1"/>
-        <v>46.761099401460008</v>
+        <v>46.761141250871042</v>
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="9"/>
@@ -4200,30 +4321,30 @@
       </c>
       <c r="AB9" s="42">
         <f t="shared" si="2"/>
-        <v>55530.225759636916</v>
+        <v>55530.292392408475</v>
       </c>
       <c r="AC9" s="28">
         <f t="shared" si="3"/>
-        <v>329.7127202886623</v>
+        <v>329.71311471397217</v>
       </c>
       <c r="AD9" s="10">
         <f t="shared" si="4"/>
-        <v>2.0831716935522779</v>
+        <v>2.083171696071715</v>
       </c>
       <c r="AE9" s="25">
         <v>1000000</v>
       </c>
       <c r="AF9" s="25">
         <f t="shared" si="5"/>
-        <v>68943.393114895807</v>
+        <v>68943.413790703795</v>
       </c>
       <c r="AG9" s="10">
         <f t="shared" si="6"/>
-        <v>5.4339667532165237</v>
+        <v>5.4339683850815081</v>
       </c>
       <c r="AH9" s="3">
         <f t="shared" si="7"/>
-        <v>2.0488037718553329</v>
+        <v>2.048803771669879</v>
       </c>
       <c r="AI9" s="3">
         <f t="shared" si="8"/>
@@ -4282,36 +4403,36 @@
         <v>10</v>
       </c>
       <c r="P10">
-        <v>7.8879538631493801E-2</v>
+        <v>7.8879562287106339E-2</v>
       </c>
       <c r="Q10">
-        <v>6.212690883582457E-6</v>
+        <v>6.2126927486998112E-6</v>
       </c>
       <c r="R10">
-        <v>2.049124972112272</v>
+        <v>2.0491249719699018</v>
       </c>
       <c r="S10">
-        <v>60.087047908308527</v>
+        <v>60.087120008979532</v>
       </c>
       <c r="T10">
-        <v>0.35684957475631129</v>
+        <v>0.35685000148982482</v>
       </c>
       <c r="U10">
-        <v>2.0830140693395758</v>
+        <v>2.0830140721470611</v>
       </c>
       <c r="V10">
-        <v>1.1130686728985529E-6</v>
+        <v>1.1130690053651901E-6</v>
       </c>
       <c r="W10">
-        <v>8.03167719802198E-3</v>
+        <v>8.0316796269975475E-3</v>
       </c>
       <c r="X10" s="10">
         <f t="shared" si="0"/>
-        <v>5.5815881219654928</v>
+        <v>5.5815881304335395</v>
       </c>
       <c r="Y10" s="10">
         <f t="shared" si="1"/>
-        <v>44.430268542689348</v>
+        <v>44.430308237185592</v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="9"/>
@@ -4322,30 +4443,30 @@
       </c>
       <c r="AB10" s="42">
         <f t="shared" si="2"/>
-        <v>60087.04790830853</v>
+        <v>60087.120008979531</v>
       </c>
       <c r="AC10" s="28">
         <f t="shared" si="3"/>
-        <v>356.84957475631131</v>
+        <v>356.85000148982482</v>
       </c>
       <c r="AD10" s="10">
         <f t="shared" si="4"/>
-        <v>2.0830140693395758</v>
+        <v>2.0830140721470611</v>
       </c>
       <c r="AE10" s="25">
         <v>1000000</v>
       </c>
       <c r="AF10" s="25">
         <f t="shared" si="5"/>
-        <v>78879.538631493808</v>
+        <v>78879.562287106339</v>
       </c>
       <c r="AG10" s="10">
         <f t="shared" si="6"/>
-        <v>6.2126908835824572</v>
+        <v>6.2126927486998111</v>
       </c>
       <c r="AH10" s="3">
         <f t="shared" si="7"/>
-        <v>2.049124972112272</v>
+        <v>2.0491249719699018</v>
       </c>
       <c r="AI10" s="3">
         <f t="shared" si="8"/>
@@ -4402,36 +4523,36 @@
         <v>10</v>
       </c>
       <c r="P11">
-        <v>8.8984218843690469E-2</v>
+        <v>8.8984245529650355E-2</v>
       </c>
       <c r="Q11">
-        <v>7.005064570812663E-6</v>
+        <v>7.0050666732793589E-6</v>
       </c>
       <c r="R11">
-        <v>2.04935091609702</v>
+        <v>2.049350915988462</v>
       </c>
       <c r="S11">
-        <v>64.608667568308334</v>
+        <v>64.608745094637982</v>
       </c>
       <c r="T11">
-        <v>0.38378644085897218</v>
+        <v>0.38378689964561419</v>
       </c>
       <c r="U11">
-        <v>2.08286295129954</v>
+        <v>2.0828629543800798</v>
       </c>
       <c r="V11">
-        <v>1.2537714435277619E-6</v>
+        <v>1.2537718187454151E-6</v>
       </c>
       <c r="W11">
-        <v>9.032189961560886E-3</v>
+        <v>9.0321926993488389E-3</v>
       </c>
       <c r="X11" s="10">
         <f t="shared" si="0"/>
-        <v>5.5871942266465826</v>
+        <v>5.587194231474248</v>
       </c>
       <c r="Y11" s="10">
         <f t="shared" si="1"/>
-        <v>42.490962047110074</v>
+        <v>42.490999962089234</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="9"/>
@@ -4442,30 +4563,30 @@
       </c>
       <c r="AB11" s="42">
         <f t="shared" si="2"/>
-        <v>64608.667568308338</v>
+        <v>64608.745094637983</v>
       </c>
       <c r="AC11" s="28">
         <f t="shared" si="3"/>
-        <v>383.78644085897218</v>
+        <v>383.7868996456142</v>
       </c>
       <c r="AD11" s="10">
         <f t="shared" si="4"/>
-        <v>2.08286295129954</v>
+        <v>2.0828629543800798</v>
       </c>
       <c r="AE11" s="25">
         <v>1000000</v>
       </c>
       <c r="AF11" s="25">
         <f t="shared" si="5"/>
-        <v>88984.218843690469</v>
+        <v>88984.245529650361</v>
       </c>
       <c r="AG11" s="10">
         <f t="shared" si="6"/>
-        <v>7.0050645708126629</v>
+        <v>7.0050666732793587</v>
       </c>
       <c r="AH11" s="3">
         <f t="shared" si="7"/>
-        <v>2.04935091609702</v>
+        <v>2.049350915988462</v>
       </c>
       <c r="AI11" s="3">
         <f t="shared" si="8"/>
@@ -4524,36 +4645,36 @@
         <v>10</v>
       </c>
       <c r="P12">
-        <v>0.10109571219089709</v>
+        <v>0.1010957425090383</v>
       </c>
       <c r="Q12">
-        <v>7.9551831211402972E-6</v>
+        <v>7.9551855081756687E-6</v>
       </c>
       <c r="R12">
-        <v>2.0495415016827332</v>
+        <v>2.0495415016079028</v>
       </c>
       <c r="S12">
-        <v>69.654224268512024</v>
+        <v>69.654307849191753</v>
       </c>
       <c r="T12">
-        <v>0.41386815376107411</v>
+        <v>0.41386864830093828</v>
       </c>
       <c r="U12">
-        <v>2.0826792840431891</v>
+        <v>2.082679287451116</v>
       </c>
       <c r="V12">
-        <v>1.422618038322458E-6</v>
+        <v>1.4226184646979509E-6</v>
       </c>
       <c r="W12">
-        <v>1.023400031510178E-2</v>
+        <v>1.0234003421571001E-2</v>
       </c>
       <c r="X12" s="10">
         <f t="shared" si="0"/>
-        <v>5.5919318515889183</v>
+        <v>5.5919318535379103</v>
       </c>
       <c r="Y12" s="10">
         <f t="shared" si="1"/>
-        <v>40.440506255442507</v>
+        <v>40.44054230318072</v>
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="9"/>
@@ -4564,30 +4685,30 @@
       </c>
       <c r="AB12" s="42">
         <f t="shared" si="2"/>
-        <v>69654.224268512029</v>
+        <v>69654.307849191755</v>
       </c>
       <c r="AC12" s="28">
         <f t="shared" si="3"/>
-        <v>413.8681537610741</v>
+        <v>413.86864830093828</v>
       </c>
       <c r="AD12" s="10">
         <f t="shared" si="4"/>
-        <v>2.0826792840431891</v>
+        <v>2.082679287451116</v>
       </c>
       <c r="AE12" s="25">
         <v>1000000</v>
       </c>
       <c r="AF12" s="25">
         <f t="shared" si="5"/>
-        <v>101095.71219089709</v>
+        <v>101095.7425090383</v>
       </c>
       <c r="AG12" s="10">
         <f t="shared" si="6"/>
-        <v>7.9551831211402968</v>
+        <v>7.9551855081756688</v>
       </c>
       <c r="AH12" s="3">
         <f t="shared" si="7"/>
-        <v>2.0495415016827332</v>
+        <v>2.0495415016079028</v>
       </c>
       <c r="AI12" s="3">
         <f t="shared" si="8"/>
@@ -4662,10 +4783,10 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>1.2570710247233239E-6</v>
+        <v>1.257071024723325E-6</v>
       </c>
       <c r="W13">
-        <v>1.257071024925346E-2</v>
+        <v>1.2570710249253471E-2</v>
       </c>
       <c r="X13" s="10">
         <f t="shared" si="0"/>
@@ -4766,36 +4887,36 @@
         <v>10</v>
       </c>
       <c r="P14">
-        <v>0.10391639287373269</v>
+        <v>0.1039164240377833</v>
       </c>
       <c r="Q14">
-        <v>9.1712122325981669E-6</v>
+        <v>9.17121500753135E-6</v>
       </c>
       <c r="R14">
-        <v>2.015367033845429</v>
+        <v>2.0153670331740301</v>
       </c>
       <c r="S14">
-        <v>167.57084657286731</v>
+        <v>167.57104764732341</v>
       </c>
       <c r="T14">
-        <v>0.99402401267466167</v>
+        <v>0.99402520453299215</v>
       </c>
       <c r="U14">
-        <v>2.0837320022815802</v>
+        <v>2.0837320029200481</v>
       </c>
       <c r="V14">
-        <v>1.9299815324925298E-6</v>
+        <v>1.9299818788286649E-6</v>
       </c>
       <c r="W14">
-        <v>1.6477593577150208E-2</v>
+        <v>1.6477595943200599E-2</v>
       </c>
       <c r="X14" s="10">
         <f t="shared" si="0"/>
-        <v>4.7519689065385728</v>
+        <v>4.7519694915982829</v>
       </c>
       <c r="Y14" s="10">
         <f t="shared" si="1"/>
-        <v>60.325799882155948</v>
+        <v>60.325863551908</v>
       </c>
       <c r="Z14" t="str">
         <f t="shared" si="9"/>
@@ -4806,30 +4927,30 @@
       </c>
       <c r="AB14" s="42">
         <f t="shared" si="2"/>
-        <v>167.57084657286731</v>
+        <v>167.57104764732341</v>
       </c>
       <c r="AC14" s="28">
         <f t="shared" si="3"/>
-        <v>0.99402401267466167</v>
+        <v>0.99402520453299215</v>
       </c>
       <c r="AD14" s="10">
         <f t="shared" si="4"/>
-        <v>2.0837320022815802</v>
+        <v>2.0837320029200481</v>
       </c>
       <c r="AE14" s="25">
         <v>1000000</v>
       </c>
       <c r="AF14" s="25">
         <f t="shared" si="5"/>
-        <v>103916.39287373269</v>
+        <v>103916.4240377833</v>
       </c>
       <c r="AG14" s="10">
         <f t="shared" si="6"/>
-        <v>9.1712122325981671</v>
+        <v>9.1712150075313499</v>
       </c>
       <c r="AH14" s="3">
         <f t="shared" si="7"/>
-        <v>2.015367033845429</v>
+        <v>2.0153670331740301</v>
       </c>
       <c r="AI14" s="3">
         <f t="shared" si="8"/>
@@ -4885,36 +5006,36 @@
         <v>10</v>
       </c>
       <c r="P15">
-        <v>0.20773376536251431</v>
+        <v>0.20773382766091961</v>
       </c>
       <c r="Q15">
-        <v>1.6838485812982589E-5</v>
+        <v>1.6838490886079981E-5</v>
       </c>
       <c r="R15">
-        <v>2.03754696758832</v>
+        <v>2.037546967064912</v>
       </c>
       <c r="S15">
-        <v>243.02318074401359</v>
+        <v>243.02347235651601</v>
       </c>
       <c r="T15">
-        <v>1.4417001651290631</v>
+        <v>1.441701892574915</v>
       </c>
       <c r="U15">
-        <v>2.0837017787629808</v>
+        <v>2.08370177997248</v>
       </c>
       <c r="V15">
-        <v>3.177629121368962E-6</v>
+        <v>3.177629941913367E-6</v>
       </c>
       <c r="W15">
-        <v>2.4517943426109971E-2</v>
+        <v>2.4517949270908911E-2</v>
       </c>
       <c r="X15" s="10">
         <f t="shared" si="0"/>
-        <v>5.2990720974159382</v>
+        <v>5.299072325565044</v>
       </c>
       <c r="Y15" s="10">
         <f t="shared" si="1"/>
-        <v>58.801839129531103</v>
+        <v>58.801895568220552</v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="9"/>
@@ -4925,30 +5046,30 @@
       </c>
       <c r="AB15" s="42">
         <f t="shared" si="2"/>
-        <v>243.02318074401359</v>
+        <v>243.02347235651601</v>
       </c>
       <c r="AC15" s="28">
         <f t="shared" si="3"/>
-        <v>1.4417001651290631</v>
+        <v>1.441701892574915</v>
       </c>
       <c r="AD15" s="10">
         <f t="shared" si="4"/>
-        <v>2.0837017787629808</v>
+        <v>2.08370177997248</v>
       </c>
       <c r="AE15" s="25">
         <v>1000000</v>
       </c>
       <c r="AF15" s="25">
         <f t="shared" si="5"/>
-        <v>207733.7653625143</v>
+        <v>207733.8276609196</v>
       </c>
       <c r="AG15" s="10">
         <f t="shared" si="6"/>
-        <v>16.83848581298259</v>
+        <v>16.838490886079981</v>
       </c>
       <c r="AH15" s="3">
         <f t="shared" si="7"/>
-        <v>2.03754696758832</v>
+        <v>2.037546967064912</v>
       </c>
       <c r="AI15" s="3">
         <f t="shared" si="8"/>
@@ -5004,36 +5125,36 @@
         <v>10</v>
       </c>
       <c r="P16">
-        <v>0.30438566272210388</v>
+        <v>0.30438575400597062</v>
       </c>
       <c r="Q16">
-        <v>2.4272929372400551E-5</v>
+        <v>2.4272936672686849E-5</v>
       </c>
       <c r="R16">
-        <v>2.0437938902369259</v>
+        <v>2.0437938898770271</v>
       </c>
       <c r="S16">
-        <v>300.38823621860018</v>
+        <v>300.38859666555408</v>
       </c>
       <c r="T16">
-        <v>1.7824934995705519</v>
+        <v>1.78249563409863</v>
       </c>
       <c r="U16">
-        <v>2.0835203245570568</v>
+        <v>2.0835203262492512</v>
       </c>
       <c r="V16">
-        <v>4.4530855193105658E-6</v>
+        <v>4.4530867665840744E-6</v>
       </c>
       <c r="W16">
-        <v>3.3199579071254551E-2</v>
+        <v>3.319958807960597E-2</v>
       </c>
       <c r="X16" s="10">
         <f t="shared" si="0"/>
-        <v>5.450811413152139</v>
+        <v>5.4508115258006562</v>
       </c>
       <c r="Y16" s="10">
         <f t="shared" si="1"/>
-        <v>53.690243955951303</v>
+        <v>53.69029368149274</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="9"/>
@@ -5044,30 +5165,30 @@
       </c>
       <c r="AB16" s="42">
         <f t="shared" si="2"/>
-        <v>300.38823621860018</v>
+        <v>300.38859666555408</v>
       </c>
       <c r="AC16" s="28">
         <f t="shared" si="3"/>
-        <v>1.7824934995705519</v>
+        <v>1.78249563409863</v>
       </c>
       <c r="AD16" s="10">
         <f t="shared" si="4"/>
-        <v>2.0835203245570568</v>
+        <v>2.0835203262492512</v>
       </c>
       <c r="AE16" s="25">
         <v>1000000</v>
       </c>
       <c r="AF16" s="25">
         <f t="shared" si="5"/>
-        <v>304385.66272210388</v>
+        <v>304385.75400597061</v>
       </c>
       <c r="AG16" s="10">
         <f t="shared" si="6"/>
-        <v>24.272929372400551</v>
+        <v>24.27293667268685</v>
       </c>
       <c r="AH16" s="3">
         <f t="shared" si="7"/>
-        <v>2.0437938902369259</v>
+        <v>2.0437938898770271</v>
       </c>
       <c r="AI16" s="3">
         <f t="shared" si="8"/>
@@ -5123,36 +5244,36 @@
         <v>10</v>
       </c>
       <c r="P17">
-        <v>0.39905115114721867</v>
+        <v>0.39905127082083208</v>
       </c>
       <c r="Q17">
-        <v>3.1628965441974232E-5</v>
+        <v>3.1628974945520972E-5</v>
       </c>
       <c r="R17">
-        <v>2.0463414579168582</v>
+        <v>2.046341457667924</v>
       </c>
       <c r="S17">
-        <v>349.02467461569171</v>
+        <v>349.02509342330683</v>
       </c>
       <c r="T17">
-        <v>2.0717478004683589</v>
+        <v>2.0717502799932288</v>
       </c>
       <c r="U17">
-        <v>2.0833084335495111</v>
+        <v>2.083308435693779</v>
       </c>
       <c r="V17">
-        <v>5.7370224585472716E-6</v>
+        <v>5.7370241155584088E-6</v>
       </c>
       <c r="W17">
-        <v>4.2122609051020297E-2</v>
+        <v>4.2122621068445741E-2</v>
       </c>
       <c r="X17" s="10">
         <f t="shared" si="0"/>
-        <v>5.513132582364566</v>
+        <v>5.5131326465484785</v>
       </c>
       <c r="Y17" s="10">
         <f t="shared" si="1"/>
-        <v>49.183748280145458</v>
+        <v>49.183793112655728</v>
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="9"/>
@@ -5163,30 +5284,30 @@
       </c>
       <c r="AB17" s="42">
         <f t="shared" si="2"/>
-        <v>349.02467461569171</v>
+        <v>349.02509342330683</v>
       </c>
       <c r="AC17" s="28">
         <f t="shared" si="3"/>
-        <v>2.0717478004683589</v>
+        <v>2.0717502799932288</v>
       </c>
       <c r="AD17" s="10">
         <f t="shared" si="4"/>
-        <v>2.0833084335495111</v>
+        <v>2.083308435693779</v>
       </c>
       <c r="AE17" s="25">
         <v>1000000</v>
       </c>
       <c r="AF17" s="25">
         <f t="shared" si="5"/>
-        <v>399051.15114721865</v>
+        <v>399051.27082083205</v>
       </c>
       <c r="AG17" s="10">
         <f t="shared" si="6"/>
-        <v>31.628965441974231</v>
+        <v>31.628974945520973</v>
       </c>
       <c r="AH17" s="3">
         <f t="shared" si="7"/>
-        <v>2.0463414579168582</v>
+        <v>2.046341457667924</v>
       </c>
       <c r="AI17" s="3">
         <f t="shared" si="8"/>
@@ -5242,36 +5363,36 @@
         <v>10</v>
       </c>
       <c r="P18">
-        <v>0.49487987904403252</v>
+        <v>0.4948800274562426</v>
       </c>
       <c r="Q18">
-        <v>3.9107063644682193E-5</v>
+        <v>3.910707538807167E-5</v>
       </c>
       <c r="R18">
-        <v>2.0476443482974331</v>
+        <v>2.0476443481238782</v>
       </c>
       <c r="S18">
-        <v>394.55689355717539</v>
+        <v>394.55736700058401</v>
       </c>
       <c r="T18">
-        <v>2.3427591124260121</v>
+        <v>2.3427619148192389</v>
       </c>
       <c r="U18">
-        <v>2.0830940355029899</v>
+        <v>2.0830940380716689</v>
       </c>
       <c r="V18">
-        <v>7.0524803516457129E-6</v>
+        <v>7.0524824193206923E-6</v>
       </c>
       <c r="W18">
-        <v>5.1357496758528583E-2</v>
+        <v>5.1357511772320841E-2</v>
       </c>
       <c r="X18" s="10">
         <f t="shared" si="0"/>
-        <v>5.5451503151733652</v>
+        <v>5.545150354566716</v>
       </c>
       <c r="Y18" s="10">
         <f t="shared" si="1"/>
-        <v>45.616692017547884</v>
+        <v>45.616733248394475</v>
       </c>
       <c r="Z18" t="str">
         <f t="shared" ref="Z18:Z19" si="10">A18&amp;B18</f>
@@ -5282,30 +5403,30 @@
       </c>
       <c r="AB18" s="42">
         <f t="shared" si="2"/>
-        <v>394.55689355717539</v>
+        <v>394.55736700058401</v>
       </c>
       <c r="AC18" s="28">
         <f t="shared" si="3"/>
-        <v>2.3427591124260121</v>
+        <v>2.3427619148192389</v>
       </c>
       <c r="AD18" s="10">
         <f t="shared" si="4"/>
-        <v>2.0830940355029899</v>
+        <v>2.0830940380716689</v>
       </c>
       <c r="AE18" s="25">
         <v>1000000</v>
       </c>
       <c r="AF18" s="25">
         <f t="shared" si="5"/>
-        <v>494879.87904403254</v>
+        <v>494880.02745624259</v>
       </c>
       <c r="AG18" s="10">
         <f t="shared" si="6"/>
-        <v>39.107063644682192</v>
+        <v>39.107075388071671</v>
       </c>
       <c r="AH18" s="3">
         <f t="shared" si="7"/>
-        <v>2.0476443482974331</v>
+        <v>2.0476443481238782</v>
       </c>
       <c r="AI18" s="3">
         <f t="shared" si="8"/>
@@ -5361,36 +5482,36 @@
         <v>10</v>
       </c>
       <c r="P19">
-        <v>0.59259699569627822</v>
+        <v>0.59259717341340423</v>
       </c>
       <c r="Q19">
-        <v>4.6749348929607873E-5</v>
+        <v>4.6749362961965763E-5</v>
       </c>
       <c r="R19">
-        <v>2.048399379039636</v>
+        <v>2.0483993789207622</v>
       </c>
       <c r="S19">
-        <v>437.93496020891081</v>
+        <v>437.93548570326573</v>
       </c>
       <c r="T19">
-        <v>2.601149816070218</v>
+        <v>2.601152925948738</v>
       </c>
       <c r="U19">
-        <v>2.0828792022748428</v>
+        <v>2.0828792052509169</v>
       </c>
       <c r="V19">
-        <v>8.4024728210543821E-6</v>
+        <v>8.4024753050584649E-6</v>
       </c>
       <c r="W19">
-        <v>6.0887774292624777E-2</v>
+        <v>6.0887792329867678E-2</v>
       </c>
       <c r="X19" s="10">
         <f t="shared" ref="X19" si="11">Q19/V19</f>
-        <v>5.5637608029467618</v>
+        <v>5.5637608281718691</v>
       </c>
       <c r="Y19" s="10">
         <f t="shared" ref="Y19" si="12">T19/W19</f>
-        <v>42.720395782069019</v>
+        <v>42.720434202255973</v>
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="10"/>
@@ -5401,30 +5522,30 @@
       </c>
       <c r="AB19" s="42">
         <f t="shared" si="2"/>
-        <v>437.93496020891081</v>
+        <v>437.93548570326573</v>
       </c>
       <c r="AC19" s="28">
         <f t="shared" si="3"/>
-        <v>2.601149816070218</v>
+        <v>2.601152925948738</v>
       </c>
       <c r="AD19" s="10">
         <f t="shared" si="4"/>
-        <v>2.0828792022748428</v>
+        <v>2.0828792052509169</v>
       </c>
       <c r="AE19" s="25">
         <v>1000000</v>
       </c>
       <c r="AF19" s="25">
         <f t="shared" si="5"/>
-        <v>592596.99569627817</v>
+        <v>592597.17341340426</v>
       </c>
       <c r="AG19" s="10">
         <f t="shared" si="6"/>
-        <v>46.749348929607876</v>
+        <v>46.749362961965765</v>
       </c>
       <c r="AH19" s="3">
         <f t="shared" si="7"/>
-        <v>2.048399379039636</v>
+        <v>2.0483993789207622</v>
       </c>
       <c r="AI19" s="3">
         <f t="shared" si="8"/>
@@ -5480,36 +5601,36 @@
         <v>10</v>
       </c>
       <c r="P20">
-        <v>0.69012907425543335</v>
+        <v>0.69012928122198336</v>
       </c>
       <c r="Q20">
-        <v>5.4386958888984962E-5</v>
+        <v>5.4386975208882958E-5</v>
       </c>
       <c r="R20">
-        <v>2.048865988469859</v>
+        <v>2.0488659883913889</v>
       </c>
       <c r="S20">
-        <v>478.98986262244472</v>
+        <v>478.99043738009539</v>
       </c>
       <c r="T20">
-        <v>2.8458729978740389</v>
+        <v>2.8458763986750308</v>
       </c>
       <c r="U20">
-        <v>2.082671670636135</v>
+        <v>2.0826716739953919</v>
       </c>
       <c r="V20">
-        <v>9.7550065138165965E-6</v>
+        <v>9.7550094118842619E-6</v>
       </c>
       <c r="W20">
-        <v>7.0468208159172069E-2</v>
+        <v>7.046822919405607E-2</v>
       </c>
       <c r="X20" s="10">
         <f t="shared" ref="X20:X23" si="13">Q20/V20</f>
-        <v>5.5752867834535502</v>
+        <v>5.5752868000952196</v>
       </c>
       <c r="Y20" s="10">
         <f t="shared" ref="Y20:Y23" si="14">T20/W20</f>
-        <v>40.385204508760069</v>
+        <v>40.385240713769463</v>
       </c>
       <c r="Z20" t="str">
         <f t="shared" ref="Z20:Z23" si="15">A20&amp;B20</f>
@@ -5520,30 +5641,30 @@
       </c>
       <c r="AB20" s="42">
         <f t="shared" si="2"/>
-        <v>478.98986262244472</v>
+        <v>478.99043738009539</v>
       </c>
       <c r="AC20" s="28">
         <f t="shared" si="3"/>
-        <v>2.8458729978740389</v>
+        <v>2.8458763986750308</v>
       </c>
       <c r="AD20" s="10">
         <f t="shared" si="4"/>
-        <v>2.082671670636135</v>
+        <v>2.0826716739953919</v>
       </c>
       <c r="AE20" s="25">
         <v>1000000</v>
       </c>
       <c r="AF20" s="25">
         <f t="shared" si="5"/>
-        <v>690129.0742554334</v>
+        <v>690129.28122198337</v>
       </c>
       <c r="AG20" s="10">
         <f t="shared" si="6"/>
-        <v>54.386958888984964</v>
+        <v>54.386975208882959</v>
       </c>
       <c r="AH20" s="3">
         <f t="shared" si="7"/>
-        <v>2.048865988469859</v>
+        <v>2.0488659883913889</v>
       </c>
       <c r="AI20" s="3">
         <f t="shared" si="8"/>
@@ -5597,36 +5718,36 @@
         <v>10</v>
       </c>
       <c r="P21">
-        <v>0.78349429499937151</v>
+        <v>0.78349452996572388</v>
       </c>
       <c r="Q21">
-        <v>6.1704115925691929E-5</v>
+        <v>6.1704134437238472E-5</v>
       </c>
       <c r="R21">
-        <v>2.0491637162439869</v>
+        <v>2.0491637161945921</v>
       </c>
       <c r="S21">
-        <v>517.38257683017093</v>
+        <v>517.38319765665926</v>
       </c>
       <c r="T21">
-        <v>3.0748269468457039</v>
+        <v>3.07483061964939</v>
       </c>
       <c r="U21">
-        <v>2.082486182258422</v>
+        <v>2.0824861859548118</v>
       </c>
       <c r="V21">
-        <v>1.1052832094483809E-5</v>
+        <v>1.105283538809727E-5</v>
       </c>
       <c r="W21">
-        <v>7.9681349143469263E-2</v>
+        <v>7.968137303737366E-2</v>
       </c>
       <c r="X21" s="10">
         <f t="shared" si="13"/>
-        <v>5.5826520658435497</v>
+        <v>5.5826520771029733</v>
       </c>
       <c r="Y21" s="10">
         <f t="shared" si="14"/>
-        <v>38.589042227552682</v>
+        <v>38.589076749558203</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="15"/>
@@ -5637,30 +5758,30 @@
       </c>
       <c r="AB21" s="42">
         <f t="shared" si="2"/>
-        <v>517.38257683017093</v>
+        <v>517.38319765665926</v>
       </c>
       <c r="AC21" s="28">
         <f t="shared" si="3"/>
-        <v>3.0748269468457039</v>
+        <v>3.07483061964939</v>
       </c>
       <c r="AD21" s="10">
         <f t="shared" si="4"/>
-        <v>2.082486182258422</v>
+        <v>2.0824861859548118</v>
       </c>
       <c r="AE21" s="25">
         <v>1000000</v>
       </c>
       <c r="AF21" s="25">
         <f t="shared" si="5"/>
-        <v>783494.29499937152</v>
+        <v>783494.52996572386</v>
       </c>
       <c r="AG21" s="10">
         <f t="shared" si="6"/>
-        <v>61.70411592569193</v>
+        <v>61.704134437238473</v>
       </c>
       <c r="AH21" s="3">
         <f t="shared" si="7"/>
-        <v>2.0491637162439869</v>
+        <v>2.0491637161945921</v>
       </c>
       <c r="AI21" s="3">
         <f t="shared" si="8"/>
@@ -5714,36 +5835,36 @@
         <v>10</v>
       </c>
       <c r="P22">
-        <v>0.87876790861691367</v>
+        <v>0.87876817215538638</v>
       </c>
       <c r="Q22">
-        <v>6.9174796536833113E-5</v>
+        <v>6.9174817286042132E-5</v>
       </c>
       <c r="R22">
-        <v>2.0493775917497081</v>
+        <v>2.049377591723657</v>
       </c>
       <c r="S22">
-        <v>555.63128085696678</v>
+        <v>555.63194757948952</v>
       </c>
       <c r="T22">
-        <v>3.3030191755949838</v>
+        <v>3.3030231193260322</v>
       </c>
       <c r="U22">
-        <v>2.0823077291212968</v>
+        <v>2.0823077331379429</v>
       </c>
       <c r="V22">
-        <v>1.237928121559361E-5</v>
+        <v>1.237928491224566E-5</v>
       </c>
       <c r="W22">
-        <v>8.9111494421127313E-2</v>
+        <v>8.9111521224561938E-2</v>
       </c>
       <c r="X22" s="10">
         <f t="shared" si="13"/>
-        <v>5.5879493592646403</v>
+        <v>5.5879493667371696</v>
       </c>
       <c r="Y22" s="10">
         <f t="shared" si="14"/>
-        <v>37.066140536095375</v>
+        <v>37.066173643275377</v>
       </c>
       <c r="Z22" t="str">
         <f t="shared" si="15"/>
@@ -5754,30 +5875,30 @@
       </c>
       <c r="AB22" s="42">
         <f t="shared" si="2"/>
-        <v>555.63128085696678</v>
+        <v>555.63194757948952</v>
       </c>
       <c r="AC22" s="28">
         <f t="shared" si="3"/>
-        <v>3.3030191755949838</v>
+        <v>3.3030231193260322</v>
       </c>
       <c r="AD22" s="10">
         <f t="shared" si="4"/>
-        <v>2.0823077291212968</v>
+        <v>2.0823077331379429</v>
       </c>
       <c r="AE22" s="25">
         <v>1000000</v>
       </c>
       <c r="AF22" s="25">
         <f t="shared" si="5"/>
-        <v>878767.90861691372</v>
+        <v>878768.17215538642</v>
       </c>
       <c r="AG22" s="10">
         <f t="shared" si="6"/>
-        <v>69.174796536833114</v>
+        <v>69.174817286042128</v>
       </c>
       <c r="AH22" s="3">
         <f t="shared" si="7"/>
-        <v>2.0493775917497081</v>
+        <v>2.049377591723657</v>
       </c>
       <c r="AI22" s="3">
         <f t="shared" si="8"/>
@@ -5831,36 +5952,36 @@
         <v>10</v>
       </c>
       <c r="P23">
-        <v>0.98565091221554635</v>
+        <v>0.98565120780774285</v>
       </c>
       <c r="Q23">
-        <v>7.7559047846046753E-5</v>
+        <v>7.7559071106422027E-5</v>
       </c>
       <c r="R23">
-        <v>2.04955001955733</v>
+        <v>2.0495500195530409</v>
       </c>
       <c r="S23">
-        <v>596.47116806980625</v>
+        <v>596.47188379762019</v>
       </c>
       <c r="T23">
-        <v>3.5468449748787378</v>
+        <v>3.5468492077880591</v>
       </c>
       <c r="U23">
-        <v>2.0821101043325649</v>
+        <v>2.0821101086991121</v>
       </c>
       <c r="V23">
-        <v>1.386908400880124E-5</v>
+        <v>1.386908815699293E-5</v>
       </c>
       <c r="W23">
-        <v>9.9713725459287528E-2</v>
+        <v>9.9713755517088554E-2</v>
       </c>
       <c r="X23" s="10">
         <f t="shared" si="13"/>
-        <v>5.5922256867741398</v>
+        <v>5.5922256912986734</v>
       </c>
       <c r="Y23" s="10">
         <f t="shared" si="14"/>
-        <v>35.570278399906861</v>
+        <v>35.570310128176992</v>
       </c>
       <c r="Z23" t="str">
         <f t="shared" si="15"/>
@@ -5871,30 +5992,30 @@
       </c>
       <c r="AB23" s="42">
         <f t="shared" si="2"/>
-        <v>596.47116806980625</v>
+        <v>596.47188379762019</v>
       </c>
       <c r="AC23" s="28">
         <f t="shared" si="3"/>
-        <v>3.5468449748787378</v>
+        <v>3.5468492077880591</v>
       </c>
       <c r="AD23" s="10">
         <f t="shared" si="4"/>
-        <v>2.0821101043325649</v>
+        <v>2.0821101086991121</v>
       </c>
       <c r="AE23" s="25">
         <v>1000000</v>
       </c>
       <c r="AF23" s="25">
         <f t="shared" si="5"/>
-        <v>985650.91221554636</v>
+        <v>985651.20780774287</v>
       </c>
       <c r="AG23" s="10">
         <f t="shared" si="6"/>
-        <v>77.559047846046752</v>
+        <v>77.559071106422024</v>
       </c>
       <c r="AH23" s="3">
         <f t="shared" si="7"/>
-        <v>2.04955001955733</v>
+        <v>2.0495500195530409</v>
       </c>
       <c r="AI23" s="3">
         <f t="shared" si="8"/>
@@ -5912,8 +6033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC1CAAA-3BCF-4A51-B8ED-6F1D21918E0E}">
   <dimension ref="A3:I25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5957,27 +6078,27 @@
       </c>
       <c r="D4" s="59">
         <f t="shared" ref="D4:D13" si="0">VLOOKUP(A4, inductor1,16,FALSE)*1000</f>
-        <v>101.09571219089709</v>
+        <v>101.0957425090383</v>
       </c>
       <c r="E4" s="59">
         <f t="shared" ref="E4:E13" si="1">VLOOKUP(A4,inductor1,17,FALSE)*1000</f>
-        <v>7.9551831211402968E-3</v>
+        <v>7.9551855081756682E-3</v>
       </c>
       <c r="F4" s="58">
         <f t="shared" ref="F4:F13" si="2">VLOOKUP(A4,inductor1,18,FALSE)</f>
-        <v>2.0495415016827332</v>
+        <v>2.0495415016079028</v>
       </c>
       <c r="G4" s="60">
         <f t="shared" ref="G4:G13" si="3">VLOOKUP(A4,inductor1,19,FALSE)</f>
-        <v>69.654224268512024</v>
+        <v>69.654307849191753</v>
       </c>
       <c r="H4" s="60">
         <f t="shared" ref="H4:H13" si="4">VLOOKUP(A4,inductor1,20,FALSE)</f>
-        <v>0.41386815376107411</v>
+        <v>0.41386864830093828</v>
       </c>
       <c r="I4" s="58">
         <f t="shared" ref="I4:I13" si="5">VLOOKUP(A4,inductor1,21,FALSE)</f>
-        <v>2.0826792840431891</v>
+        <v>2.082679287451116</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5989,27 +6110,27 @@
       </c>
       <c r="D5" s="59">
         <f t="shared" si="0"/>
-        <v>88.984218843690471</v>
+        <v>88.984245529650352</v>
       </c>
       <c r="E5" s="59">
         <f t="shared" si="1"/>
-        <v>7.0050645708126628E-3</v>
+        <v>7.0050666732793592E-3</v>
       </c>
       <c r="F5" s="58">
         <f t="shared" si="2"/>
-        <v>2.04935091609702</v>
+        <v>2.049350915988462</v>
       </c>
       <c r="G5" s="60">
         <f t="shared" si="3"/>
-        <v>64.608667568308334</v>
+        <v>64.608745094637982</v>
       </c>
       <c r="H5" s="60">
         <f t="shared" si="4"/>
-        <v>0.38378644085897218</v>
+        <v>0.38378689964561419</v>
       </c>
       <c r="I5" s="58">
         <f t="shared" si="5"/>
-        <v>2.08286295129954</v>
+        <v>2.0828629543800798</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -6021,27 +6142,27 @@
       </c>
       <c r="D6" s="59">
         <f t="shared" si="0"/>
-        <v>78.879538631493801</v>
+        <v>78.879562287106339</v>
       </c>
       <c r="E6" s="59">
         <f t="shared" si="1"/>
-        <v>6.2126908835824571E-3</v>
+        <v>6.212692748699811E-3</v>
       </c>
       <c r="F6" s="58">
         <f t="shared" si="2"/>
-        <v>2.049124972112272</v>
+        <v>2.0491249719699018</v>
       </c>
       <c r="G6" s="60">
         <f t="shared" si="3"/>
-        <v>60.087047908308527</v>
+        <v>60.087120008979532</v>
       </c>
       <c r="H6" s="60">
         <f t="shared" si="4"/>
-        <v>0.35684957475631129</v>
+        <v>0.35685000148982482</v>
       </c>
       <c r="I6" s="58">
         <f t="shared" si="5"/>
-        <v>2.0830140693395758</v>
+        <v>2.0830140721470611</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -6053,27 +6174,27 @@
       </c>
       <c r="D7" s="59">
         <f t="shared" si="0"/>
-        <v>68.943393114895812</v>
+        <v>68.943413790703787</v>
       </c>
       <c r="E7" s="59">
         <f t="shared" si="1"/>
-        <v>5.433966753216524E-3</v>
+        <v>5.4339683850815083E-3</v>
       </c>
       <c r="F7" s="58">
         <f t="shared" si="2"/>
-        <v>2.0488037718553329</v>
+        <v>2.048803771669879</v>
       </c>
       <c r="G7" s="60">
         <f t="shared" si="3"/>
-        <v>55.530225759636913</v>
+        <v>55.530292392408477</v>
       </c>
       <c r="H7" s="60">
         <f t="shared" si="4"/>
-        <v>0.32971272028866228</v>
+        <v>0.32971311471397219</v>
       </c>
       <c r="I7" s="58">
         <f t="shared" si="5"/>
-        <v>2.0831716935522779</v>
+        <v>2.083171696071715</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -6085,27 +6206,27 @@
       </c>
       <c r="D8" s="59">
         <f t="shared" si="0"/>
-        <v>59.098366356571042</v>
+        <v>59.098384079900562</v>
       </c>
       <c r="E8" s="59">
         <f t="shared" si="1"/>
-        <v>4.6630188105605619E-3</v>
+        <v>4.663020211508038E-3</v>
       </c>
       <c r="F8" s="58">
         <f t="shared" si="2"/>
-        <v>2.048321446438941</v>
+        <v>2.048321446196987</v>
       </c>
       <c r="G8" s="60">
         <f t="shared" si="3"/>
-        <v>50.843894455198154</v>
+        <v>50.843955464667467</v>
       </c>
       <c r="H8" s="60">
         <f t="shared" si="4"/>
-        <v>0.30181722511744519</v>
+        <v>0.3018175863091932</v>
       </c>
       <c r="I8" s="58">
         <f t="shared" si="5"/>
-        <v>2.0833352473248459</v>
+        <v>2.0833352495406552</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -6117,27 +6238,27 @@
       </c>
       <c r="D9" s="59">
         <f t="shared" si="0"/>
-        <v>49.054898745980545</v>
+        <v>49.054913457320097</v>
       </c>
       <c r="E9" s="59">
         <f t="shared" si="1"/>
-        <v>3.877568212412065E-3</v>
+        <v>3.8775693780887248E-3</v>
       </c>
       <c r="F9" s="58">
         <f t="shared" si="2"/>
-        <v>2.0475205998446748</v>
+        <v>2.04752059952513</v>
       </c>
       <c r="G9" s="60">
         <f t="shared" si="3"/>
-        <v>45.744533951285788</v>
+        <v>45.74458884184385</v>
       </c>
       <c r="H9" s="60">
         <f t="shared" si="4"/>
-        <v>0.27148179239964138</v>
+        <v>0.2714821174183315</v>
       </c>
       <c r="I9" s="58">
         <f t="shared" si="5"/>
-        <v>2.0835047626907799</v>
+        <v>2.0835047645835121</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -6149,27 +6270,27 @@
       </c>
       <c r="D10" s="59">
         <f t="shared" si="0"/>
-        <v>39.351501144313183</v>
+        <v>39.351512945648217</v>
       </c>
       <c r="E10" s="59">
         <f t="shared" si="1"/>
-        <v>3.120455472991634E-3</v>
+        <v>3.1204564118696618E-3</v>
       </c>
       <c r="F10" s="58">
         <f t="shared" si="2"/>
-        <v>2.0461426234706419</v>
+        <v>2.046142623046403</v>
       </c>
       <c r="G10" s="60">
         <f t="shared" si="3"/>
-        <v>40.399956111511642</v>
+        <v>40.400004588913077</v>
       </c>
       <c r="H10" s="60">
         <f t="shared" si="4"/>
-        <v>0.23970869198841849</v>
+        <v>0.23970897908311969</v>
       </c>
       <c r="I10" s="58">
         <f t="shared" si="5"/>
-        <v>2.0836682469806882</v>
+        <v>2.0836682485476938</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -6181,27 +6302,27 @@
       </c>
       <c r="D11" s="59">
         <f t="shared" si="0"/>
-        <v>29.269025503287381</v>
+        <v>29.26903428093414</v>
       </c>
       <c r="E11" s="59">
         <f t="shared" si="1"/>
-        <v>2.3374466022814499E-3</v>
+        <v>2.3374473066053911E-3</v>
       </c>
       <c r="F11" s="58">
         <f t="shared" si="2"/>
-        <v>2.0431969812943169</v>
+        <v>2.0431969807060941</v>
       </c>
       <c r="G11" s="60">
         <f t="shared" si="3"/>
-        <v>34.345528088235419</v>
+        <v>34.345569300704767</v>
       </c>
       <c r="H11" s="60">
         <f t="shared" si="4"/>
-        <v>0.2037388544346653</v>
+        <v>0.20373909855685571</v>
       </c>
       <c r="I11" s="58">
         <f t="shared" si="5"/>
-        <v>2.0838364610538198</v>
+        <v>2.083836462257691</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -6213,27 +6334,27 @@
       </c>
       <c r="D12" s="59">
         <f t="shared" si="0"/>
-        <v>19.991315536319089</v>
+        <v>19.9913215316231</v>
       </c>
       <c r="E12" s="59">
         <f t="shared" si="1"/>
-        <v>1.6250152697106631E-3</v>
+        <v>1.625015760574233E-3</v>
       </c>
       <c r="F12" s="58">
         <f t="shared" si="2"/>
-        <v>2.036544885767873</v>
+        <v>2.0365448849629679</v>
       </c>
       <c r="G12" s="60">
         <f t="shared" si="3"/>
-        <v>27.90327264714842</v>
+        <v>27.903306129317219</v>
       </c>
       <c r="H12" s="60">
         <f t="shared" si="4"/>
-        <v>0.1654960414164828</v>
+        <v>0.16549623979952069</v>
       </c>
       <c r="I12" s="58">
         <f t="shared" si="5"/>
-        <v>2.083965226242531</v>
+        <v>2.08396522709607</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -6245,27 +6366,27 @@
       </c>
       <c r="D13" s="59">
         <f t="shared" si="0"/>
-        <v>10.151089766355591</v>
+        <v>10.151092810620941</v>
       </c>
       <c r="E13" s="59">
         <f t="shared" si="1"/>
-        <v>9.0104883355186143E-4</v>
+        <v>9.0104910728435296E-4</v>
       </c>
       <c r="F13" s="58">
         <f t="shared" si="2"/>
-        <v>2.0142871658839789</v>
+        <v>2.0142871649350962</v>
       </c>
       <c r="G13" s="60">
         <f t="shared" si="3"/>
-        <v>19.40867211366508</v>
+        <v>19.40869540284854</v>
       </c>
       <c r="H13" s="60">
         <f t="shared" si="4"/>
-        <v>0.11511800312028141</v>
+        <v>0.1151181411798763</v>
       </c>
       <c r="I13" s="58">
         <f t="shared" si="5"/>
-        <v>2.0839745776262251</v>
+        <v>2.083974578081909</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6300,27 +6421,27 @@
       </c>
       <c r="D16" s="61">
         <f t="shared" ref="D16:D25" si="6">VLOOKUP(A16, inductor2,16,FALSE)*1000</f>
-        <v>985.65091221554633</v>
+        <v>985.65120780774282</v>
       </c>
       <c r="E16" s="61">
         <f t="shared" ref="E16:E25" si="7">VLOOKUP(A16,inductor2,17,FALSE)*1000</f>
-        <v>7.7559047846046753E-2</v>
+        <v>7.7559071106422031E-2</v>
       </c>
       <c r="F16" s="58">
         <f t="shared" ref="F16:F25" si="8">VLOOKUP(A16,inductor2,18,FALSE)</f>
-        <v>2.04955001955733</v>
+        <v>2.0495500195530409</v>
       </c>
       <c r="G16" s="62">
         <f t="shared" ref="G16:G25" si="9">VLOOKUP(A16,inductor2,19,FALSE)</f>
-        <v>596.47116806980625</v>
+        <v>596.47188379762019</v>
       </c>
       <c r="H16" s="62">
         <f t="shared" ref="H16:H25" si="10">VLOOKUP(A16,inductor2,20,FALSE)</f>
-        <v>3.5468449748787378</v>
+        <v>3.5468492077880591</v>
       </c>
       <c r="I16" s="58">
         <f t="shared" ref="I16:I25" si="11">VLOOKUP(A16,inductor2,21,FALSE)</f>
-        <v>2.0821101043325649</v>
+        <v>2.0821101086991121</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -6332,27 +6453,27 @@
       </c>
       <c r="D17" s="61">
         <f t="shared" si="6"/>
-        <v>878.7679086169137</v>
+        <v>878.76817215538642</v>
       </c>
       <c r="E17" s="61">
         <f t="shared" si="7"/>
-        <v>6.9174796536833116E-2</v>
+        <v>6.9174817286042134E-2</v>
       </c>
       <c r="F17" s="58">
         <f t="shared" si="8"/>
-        <v>2.0493775917497081</v>
+        <v>2.049377591723657</v>
       </c>
       <c r="G17" s="62">
         <f t="shared" si="9"/>
-        <v>555.63128085696678</v>
+        <v>555.63194757948952</v>
       </c>
       <c r="H17" s="62">
         <f t="shared" si="10"/>
-        <v>3.3030191755949838</v>
+        <v>3.3030231193260322</v>
       </c>
       <c r="I17" s="58">
         <f t="shared" si="11"/>
-        <v>2.0823077291212968</v>
+        <v>2.0823077331379429</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -6364,27 +6485,27 @@
       </c>
       <c r="D18" s="61">
         <f t="shared" si="6"/>
-        <v>783.4942949993715</v>
+        <v>783.49452996572393</v>
       </c>
       <c r="E18" s="61">
         <f t="shared" si="7"/>
-        <v>6.170411592569193E-2</v>
+        <v>6.1704134437238475E-2</v>
       </c>
       <c r="F18" s="58">
         <f t="shared" si="8"/>
-        <v>2.0491637162439869</v>
+        <v>2.0491637161945921</v>
       </c>
       <c r="G18" s="62">
         <f t="shared" si="9"/>
-        <v>517.38257683017093</v>
+        <v>517.38319765665926</v>
       </c>
       <c r="H18" s="62">
         <f t="shared" si="10"/>
-        <v>3.0748269468457039</v>
+        <v>3.07483061964939</v>
       </c>
       <c r="I18" s="58">
         <f t="shared" si="11"/>
-        <v>2.082486182258422</v>
+        <v>2.0824861859548118</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -6396,27 +6517,27 @@
       </c>
       <c r="D19" s="61">
         <f t="shared" si="6"/>
-        <v>690.12907425543335</v>
+        <v>690.12928122198332</v>
       </c>
       <c r="E19" s="61">
         <f t="shared" si="7"/>
-        <v>5.4386958888984961E-2</v>
+        <v>5.4386975208882957E-2</v>
       </c>
       <c r="F19" s="58">
         <f t="shared" si="8"/>
-        <v>2.048865988469859</v>
+        <v>2.0488659883913889</v>
       </c>
       <c r="G19" s="62">
         <f t="shared" si="9"/>
-        <v>478.98986262244472</v>
+        <v>478.99043738009539</v>
       </c>
       <c r="H19" s="62">
         <f t="shared" si="10"/>
-        <v>2.8458729978740389</v>
+        <v>2.8458763986750308</v>
       </c>
       <c r="I19" s="58">
         <f t="shared" si="11"/>
-        <v>2.082671670636135</v>
+        <v>2.0826716739953919</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -6428,27 +6549,27 @@
       </c>
       <c r="D20" s="61">
         <f t="shared" si="6"/>
-        <v>592.59699569627821</v>
+        <v>592.59717341340422</v>
       </c>
       <c r="E20" s="61">
         <f t="shared" si="7"/>
-        <v>4.6749348929607873E-2</v>
+        <v>4.674936296196576E-2</v>
       </c>
       <c r="F20" s="58">
         <f t="shared" si="8"/>
-        <v>2.048399379039636</v>
+        <v>2.0483993789207622</v>
       </c>
       <c r="G20" s="62">
         <f t="shared" si="9"/>
-        <v>437.93496020891081</v>
+        <v>437.93548570326573</v>
       </c>
       <c r="H20" s="62">
         <f t="shared" si="10"/>
-        <v>2.601149816070218</v>
+        <v>2.601152925948738</v>
       </c>
       <c r="I20" s="58">
         <f t="shared" si="11"/>
-        <v>2.0828792022748428</v>
+        <v>2.0828792052509169</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -6460,27 +6581,27 @@
       </c>
       <c r="D21" s="61">
         <f t="shared" si="6"/>
-        <v>494.87987904403252</v>
+        <v>494.8800274562426</v>
       </c>
       <c r="E21" s="61">
         <f t="shared" si="7"/>
-        <v>3.9107063644682194E-2</v>
+        <v>3.910707538807167E-2</v>
       </c>
       <c r="F21" s="58">
         <f t="shared" si="8"/>
-        <v>2.0476443482974331</v>
+        <v>2.0476443481238782</v>
       </c>
       <c r="G21" s="62">
         <f t="shared" si="9"/>
-        <v>394.55689355717539</v>
+        <v>394.55736700058401</v>
       </c>
       <c r="H21" s="62">
         <f t="shared" si="10"/>
-        <v>2.3427591124260121</v>
+        <v>2.3427619148192389</v>
       </c>
       <c r="I21" s="58">
         <f t="shared" si="11"/>
-        <v>2.0830940355029899</v>
+        <v>2.0830940380716689</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -6492,27 +6613,27 @@
       </c>
       <c r="D22" s="61">
         <f t="shared" si="6"/>
-        <v>399.05115114721866</v>
+        <v>399.05127082083209</v>
       </c>
       <c r="E22" s="61">
         <f t="shared" si="7"/>
-        <v>3.162896544197423E-2</v>
+        <v>3.1628974945520971E-2</v>
       </c>
       <c r="F22" s="58">
         <f t="shared" si="8"/>
-        <v>2.0463414579168582</v>
+        <v>2.046341457667924</v>
       </c>
       <c r="G22" s="62">
         <f t="shared" si="9"/>
-        <v>349.02467461569171</v>
+        <v>349.02509342330683</v>
       </c>
       <c r="H22" s="62">
         <f t="shared" si="10"/>
-        <v>2.0717478004683589</v>
+        <v>2.0717502799932288</v>
       </c>
       <c r="I22" s="58">
         <f t="shared" si="11"/>
-        <v>2.0833084335495111</v>
+        <v>2.083308435693779</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -6524,27 +6645,27 @@
       </c>
       <c r="D23" s="61">
         <f t="shared" si="6"/>
-        <v>304.38566272210386</v>
+        <v>304.38575400597063</v>
       </c>
       <c r="E23" s="61">
         <f t="shared" si="7"/>
-        <v>2.427292937240055E-2</v>
+        <v>2.4272936672686849E-2</v>
       </c>
       <c r="F23" s="58">
         <f t="shared" si="8"/>
-        <v>2.0437938902369259</v>
+        <v>2.0437938898770271</v>
       </c>
       <c r="G23" s="62">
         <f t="shared" si="9"/>
-        <v>300.38823621860018</v>
+        <v>300.38859666555408</v>
       </c>
       <c r="H23" s="62">
         <f t="shared" si="10"/>
-        <v>1.7824934995705519</v>
+        <v>1.78249563409863</v>
       </c>
       <c r="I23" s="58">
         <f t="shared" si="11"/>
-        <v>2.0835203245570568</v>
+        <v>2.0835203262492512</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -6556,27 +6677,27 @@
       </c>
       <c r="D24" s="61">
         <f t="shared" si="6"/>
-        <v>207.7337653625143</v>
+        <v>207.73382766091962</v>
       </c>
       <c r="E24" s="61">
         <f t="shared" si="7"/>
-        <v>1.6838485812982588E-2</v>
+        <v>1.6838490886079981E-2</v>
       </c>
       <c r="F24" s="58">
         <f t="shared" si="8"/>
-        <v>2.03754696758832</v>
+        <v>2.037546967064912</v>
       </c>
       <c r="G24" s="62">
         <f t="shared" si="9"/>
-        <v>243.02318074401359</v>
+        <v>243.02347235651601</v>
       </c>
       <c r="H24" s="62">
         <f t="shared" si="10"/>
-        <v>1.4417001651290631</v>
+        <v>1.441701892574915</v>
       </c>
       <c r="I24" s="58">
         <f t="shared" si="11"/>
-        <v>2.0837017787629808</v>
+        <v>2.08370177997248</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -6588,27 +6709,27 @@
       </c>
       <c r="D25" s="61">
         <f t="shared" si="6"/>
-        <v>103.91639287373269</v>
+        <v>103.9164240377833</v>
       </c>
       <c r="E25" s="61">
         <f t="shared" si="7"/>
-        <v>9.1712122325981662E-3</v>
+        <v>9.1712150075313505E-3</v>
       </c>
       <c r="F25" s="58">
         <f t="shared" si="8"/>
-        <v>2.015367033845429</v>
+        <v>2.0153670331740301</v>
       </c>
       <c r="G25" s="62">
         <f t="shared" si="9"/>
-        <v>167.57084657286731</v>
+        <v>167.57104764732341</v>
       </c>
       <c r="H25" s="62">
         <f t="shared" si="10"/>
-        <v>0.99402401267466167</v>
+        <v>0.99402520453299215</v>
       </c>
       <c r="I25" s="58">
         <f t="shared" si="11"/>
-        <v>2.0837320022815802</v>
+        <v>2.0837320029200481</v>
       </c>
     </row>
   </sheetData>
@@ -6618,6 +6739,556 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B721CEED-5171-447F-A677-E8AEDA9EEDF1}">
+  <dimension ref="B3:I68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="65.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <v>0.120486588288272</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6">
+        <v>0.12043166848900801</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>1.33294898445812E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8">
+        <v>1.20186496693308E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9">
+        <v>1.1776113995447799E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10">
+        <v>1.1776113995447799E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11">
+        <v>1.0000707009045599E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12">
+        <v>1.0000707009045599E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13">
+        <v>8.4120941741272796E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14">
+        <v>1.5021761977077099E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>1.5021761977077099E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16">
+        <v>1.5021761977077099E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="25">
+        <v>6.0087047908308501E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="25">
+        <v>6.0087047908308501E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="25">
+        <v>6.0087047908308501E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="25">
+        <v>6.0087047908308501E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="25">
+        <v>6.0087047908308501E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="25">
+        <v>6.0087047908308501E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="25">
+        <v>4.2487959037445902E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="25">
+        <v>3.0043271590672901E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="25">
+        <v>3.0043109359245099E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="25">
+        <v>3.0041892679381701E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="25">
+        <v>1.2431840226785001E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="25">
+        <v>1.2400876691216501E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="25">
+        <v>1.9769122898460399E-6</v>
+      </c>
+      <c r="I38" s="25"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="25">
+        <v>1.92113603318284E-6</v>
+      </c>
+      <c r="I39" s="25"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="25">
+        <v>1.10430139352558E-6</v>
+      </c>
+      <c r="I40" s="25"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="25">
+        <v>3.9439769315746902E-7</v>
+      </c>
+      <c r="I41" s="25"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="25">
+        <v>1.9719884657873401E-7</v>
+      </c>
+      <c r="I42" s="25"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="25">
+        <v>1.9719884657873401E-7</v>
+      </c>
+      <c r="I43" s="25"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="25">
+        <v>1.9719884657873401E-7</v>
+      </c>
+      <c r="I44" s="25"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="25">
+        <v>1.17777061040889E-7</v>
+      </c>
+      <c r="I45" s="25"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="25">
+        <v>1.17777061040889E-7</v>
+      </c>
+      <c r="I46" s="25"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="25">
+        <v>1.01608476085572E-7</v>
+      </c>
+      <c r="I47" s="25"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" s="25">
+        <v>1.0002059085974499E-7</v>
+      </c>
+      <c r="I48" s="25"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" s="25">
+        <v>1.0002059085974499E-7</v>
+      </c>
+      <c r="I49" s="25"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="25">
+        <v>7.8879538631493801E-8</v>
+      </c>
+      <c r="I50" s="25"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="25">
+        <v>7.8879538631493801E-8</v>
+      </c>
+      <c r="I51" s="25"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="25">
+        <v>7.8879538631493801E-8</v>
+      </c>
+      <c r="I52" s="25"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="25">
+        <v>7.8879538631493801E-8</v>
+      </c>
+      <c r="I53" s="25"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="25">
+        <v>7.8879538631493801E-8</v>
+      </c>
+      <c r="I54" s="25"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="25">
+        <v>7.8867787331181396E-8</v>
+      </c>
+      <c r="I55" s="25"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="25">
+        <v>5.5776256663195502E-8</v>
+      </c>
+      <c r="I56" s="25"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="25">
+        <v>3.94394380244675E-8</v>
+      </c>
+      <c r="I57" s="25"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="25">
+        <v>3.9437627852554499E-8</v>
+      </c>
+      <c r="I58" s="25"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>100</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>127</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I576"/>
   <sheetViews>
@@ -10741,7 +11412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>

</xml_diff>